<commit_message>
branch pipeline have done, need to do bubble pipeline, including source register(have done), data check, datapath
</commit_message>
<xml_diff>
--- a/CPU28/单周期控制器2020-2-14.xlsx
+++ b/CPU28/单周期控制器2020-2-14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21360" windowHeight="9684"/>
+    <workbookView windowWidth="16331" windowHeight="9684"/>
   </bookViews>
   <sheets>
     <sheet name="真值表" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="122">
   <si>
     <t>#</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>BLTZ</t>
+  </si>
+  <si>
+    <t>R1_Used</t>
+  </si>
+  <si>
+    <t>R2_Used</t>
   </si>
   <si>
     <t>XXX</t>
@@ -836,10 +842,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="51">
     <font>
@@ -1007,12 +1013,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -1027,25 +1048,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1060,6 +1067,38 @@
       <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1079,57 +1118,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1143,8 +1134,23 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1198,7 +1204,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1261,7 +1267,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1273,73 +1411,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1357,67 +1429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1429,19 +1441,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1629,36 +1629,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1680,15 +1650,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1712,16 +1697,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1732,10 +1732,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1744,133 +1744,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="23" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="30" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="30" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="28" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="37" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2454,8 +2454,8 @@
   </sheetPr>
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="W30" sqref="W30"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AL13" sqref="AL13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -2589,28 +2589,28 @@
         <v>35</v>
       </c>
       <c r="AK1" s="42" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AL1" s="42" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AM1" s="42" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AN1" s="42" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AO1" s="42" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AP1" s="42" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AQ1" s="42" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AR1" s="42" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:44">
@@ -2618,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="54">
         <v>0</v>
@@ -2712,7 +2712,9 @@
       <c r="AH2" s="54"/>
       <c r="AI2" s="54"/>
       <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
+      <c r="AK2" s="54">
+        <v>1</v>
+      </c>
       <c r="AL2" s="54"/>
       <c r="AM2" s="54"/>
       <c r="AN2" s="54"/>
@@ -2726,7 +2728,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" s="28">
         <v>0</v>
@@ -2820,7 +2822,9 @@
       <c r="AH3" s="65"/>
       <c r="AI3" s="65"/>
       <c r="AJ3" s="65"/>
-      <c r="AK3" s="65"/>
+      <c r="AK3" s="65">
+        <v>1</v>
+      </c>
       <c r="AL3" s="65"/>
       <c r="AM3" s="65"/>
       <c r="AN3" s="65"/>
@@ -2834,7 +2838,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C4" s="54">
         <v>0</v>
@@ -2928,7 +2932,9 @@
       <c r="AH4" s="54"/>
       <c r="AI4" s="54"/>
       <c r="AJ4" s="54"/>
-      <c r="AK4" s="54"/>
+      <c r="AK4" s="54">
+        <v>1</v>
+      </c>
       <c r="AL4" s="54"/>
       <c r="AM4" s="54"/>
       <c r="AN4" s="54"/>
@@ -2942,7 +2948,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" s="28">
         <v>0</v>
@@ -3035,8 +3041,12 @@
       <c r="AG5" s="27"/>
       <c r="AH5" s="65"/>
       <c r="AI5" s="65"/>
-      <c r="AJ5" s="65"/>
-      <c r="AK5" s="65"/>
+      <c r="AJ5" s="65">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="65">
+        <v>1</v>
+      </c>
       <c r="AL5" s="65"/>
       <c r="AM5" s="65"/>
       <c r="AN5" s="65"/>
@@ -3050,7 +3060,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" s="54">
         <v>0</v>
@@ -3143,8 +3153,12 @@
       <c r="AG6" s="53"/>
       <c r="AH6" s="54"/>
       <c r="AI6" s="54"/>
-      <c r="AJ6" s="54"/>
-      <c r="AK6" s="54"/>
+      <c r="AJ6" s="54">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="54">
+        <v>1</v>
+      </c>
       <c r="AL6" s="54"/>
       <c r="AM6" s="54"/>
       <c r="AN6" s="54"/>
@@ -3158,7 +3172,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7" s="28">
         <v>0</v>
@@ -3251,8 +3265,12 @@
       <c r="AG7" s="27"/>
       <c r="AH7" s="65"/>
       <c r="AI7" s="65"/>
-      <c r="AJ7" s="65"/>
-      <c r="AK7" s="65"/>
+      <c r="AJ7" s="65">
+        <v>1</v>
+      </c>
+      <c r="AK7" s="65">
+        <v>1</v>
+      </c>
       <c r="AL7" s="65"/>
       <c r="AM7" s="65"/>
       <c r="AN7" s="65"/>
@@ -3266,7 +3284,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C8" s="54">
         <v>0</v>
@@ -3359,8 +3377,12 @@
       <c r="AG8" s="53"/>
       <c r="AH8" s="54"/>
       <c r="AI8" s="54"/>
-      <c r="AJ8" s="54"/>
-      <c r="AK8" s="54"/>
+      <c r="AJ8" s="54">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="54">
+        <v>1</v>
+      </c>
       <c r="AL8" s="54"/>
       <c r="AM8" s="54"/>
       <c r="AN8" s="54"/>
@@ -3374,7 +3396,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" s="28">
         <v>0</v>
@@ -3467,8 +3489,12 @@
       <c r="AG9" s="27"/>
       <c r="AH9" s="65"/>
       <c r="AI9" s="65"/>
-      <c r="AJ9" s="65"/>
-      <c r="AK9" s="65"/>
+      <c r="AJ9" s="65">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="65">
+        <v>1</v>
+      </c>
       <c r="AL9" s="65"/>
       <c r="AM9" s="65"/>
       <c r="AN9" s="65"/>
@@ -3482,7 +3508,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" s="54">
         <v>0</v>
@@ -3575,8 +3601,12 @@
       <c r="AG10" s="53"/>
       <c r="AH10" s="54"/>
       <c r="AI10" s="54"/>
-      <c r="AJ10" s="54"/>
-      <c r="AK10" s="54"/>
+      <c r="AJ10" s="54">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="54">
+        <v>1</v>
+      </c>
       <c r="AL10" s="54"/>
       <c r="AM10" s="54"/>
       <c r="AN10" s="54"/>
@@ -3590,7 +3620,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="28">
         <v>0</v>
@@ -3683,8 +3713,12 @@
       <c r="AG11" s="27"/>
       <c r="AH11" s="65"/>
       <c r="AI11" s="65"/>
-      <c r="AJ11" s="65"/>
-      <c r="AK11" s="65"/>
+      <c r="AJ11" s="65">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="65">
+        <v>1</v>
+      </c>
       <c r="AL11" s="65"/>
       <c r="AM11" s="65"/>
       <c r="AN11" s="65"/>
@@ -3698,7 +3732,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C12" s="54">
         <v>0</v>
@@ -3791,8 +3825,12 @@
       <c r="AG12" s="53"/>
       <c r="AH12" s="54"/>
       <c r="AI12" s="54"/>
-      <c r="AJ12" s="54"/>
-      <c r="AK12" s="54"/>
+      <c r="AJ12" s="54">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="54">
+        <v>1</v>
+      </c>
       <c r="AL12" s="54"/>
       <c r="AM12" s="54"/>
       <c r="AN12" s="54"/>
@@ -3863,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="63" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R13" s="64" t="str">
         <f t="shared" si="12"/>
@@ -3899,7 +3937,9 @@
       <c r="AG13" s="27"/>
       <c r="AH13" s="65"/>
       <c r="AI13" s="65"/>
-      <c r="AJ13" s="65"/>
+      <c r="AJ13" s="65">
+        <v>1</v>
+      </c>
       <c r="AK13" s="65"/>
       <c r="AL13" s="65"/>
       <c r="AM13" s="65"/>
@@ -3971,7 +4011,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="61" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R14" s="62" t="str">
         <f t="shared" si="12"/>
@@ -4005,8 +4045,12 @@
       <c r="AG14" s="53"/>
       <c r="AH14" s="54"/>
       <c r="AI14" s="54"/>
-      <c r="AJ14" s="54"/>
-      <c r="AK14" s="54"/>
+      <c r="AJ14" s="54">
+        <v>1</v>
+      </c>
+      <c r="AK14" s="54">
+        <v>1</v>
+      </c>
       <c r="AL14" s="54"/>
       <c r="AM14" s="54"/>
       <c r="AN14" s="54"/>
@@ -4020,13 +4064,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="56" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C15" s="28">
         <v>2</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E15" s="57">
         <f t="shared" si="0"/>
@@ -4077,7 +4121,7 @@
         <v/>
       </c>
       <c r="Q15" s="63" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R15" s="64" t="str">
         <f t="shared" si="12"/>
@@ -4132,7 +4176,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="55" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E16" s="54">
         <f t="shared" si="0"/>
@@ -4183,7 +4227,7 @@
         <v/>
       </c>
       <c r="Q16" s="61" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R16" s="62" t="str">
         <f t="shared" si="12"/>
@@ -4242,7 +4286,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E17" s="57">
         <f t="shared" si="0"/>
@@ -4293,7 +4337,7 @@
         <v/>
       </c>
       <c r="Q17" s="63" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R17" s="64" t="str">
         <f t="shared" si="12"/>
@@ -4327,8 +4371,12 @@
       <c r="AG17" s="27"/>
       <c r="AH17" s="65"/>
       <c r="AI17" s="65"/>
-      <c r="AJ17" s="65"/>
-      <c r="AK17" s="65"/>
+      <c r="AJ17" s="65">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="65">
+        <v>1</v>
+      </c>
       <c r="AL17" s="65"/>
       <c r="AM17" s="65"/>
       <c r="AN17" s="65"/>
@@ -4348,7 +4396,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="55" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E18" s="54">
         <f t="shared" si="0"/>
@@ -4399,7 +4447,7 @@
         <v/>
       </c>
       <c r="Q18" s="61" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R18" s="62" t="str">
         <f t="shared" si="12"/>
@@ -4433,8 +4481,12 @@
       <c r="AG18" s="53"/>
       <c r="AH18" s="54"/>
       <c r="AI18" s="54"/>
-      <c r="AJ18" s="54"/>
-      <c r="AK18" s="54"/>
+      <c r="AJ18" s="54">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="54">
+        <v>1</v>
+      </c>
       <c r="AL18" s="54"/>
       <c r="AM18" s="54"/>
       <c r="AN18" s="54"/>
@@ -4448,13 +4500,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C19" s="28">
         <v>8</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E19" s="57">
         <f t="shared" si="0"/>
@@ -4543,7 +4595,9 @@
       <c r="AG19" s="27"/>
       <c r="AH19" s="65"/>
       <c r="AI19" s="65"/>
-      <c r="AJ19" s="65"/>
+      <c r="AJ19" s="65">
+        <v>1</v>
+      </c>
       <c r="AK19" s="65"/>
       <c r="AL19" s="65"/>
       <c r="AM19" s="65"/>
@@ -4558,13 +4612,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C20" s="54">
         <v>12</v>
       </c>
       <c r="D20" s="55" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E20" s="54">
         <f t="shared" si="0"/>
@@ -4651,7 +4705,9 @@
       <c r="AG20" s="53"/>
       <c r="AH20" s="54"/>
       <c r="AI20" s="54"/>
-      <c r="AJ20" s="54"/>
+      <c r="AJ20" s="54">
+        <v>1</v>
+      </c>
       <c r="AK20" s="54"/>
       <c r="AL20" s="54"/>
       <c r="AM20" s="54"/>
@@ -4666,13 +4722,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="56" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" s="28">
         <v>9</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E21" s="57">
         <f t="shared" si="0"/>
@@ -4761,7 +4817,9 @@
       <c r="AG21" s="27"/>
       <c r="AH21" s="65"/>
       <c r="AI21" s="65"/>
-      <c r="AJ21" s="65"/>
+      <c r="AJ21" s="65">
+        <v>1</v>
+      </c>
       <c r="AK21" s="65"/>
       <c r="AL21" s="65"/>
       <c r="AM21" s="65"/>
@@ -4776,13 +4834,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C22" s="54">
         <v>10</v>
       </c>
       <c r="D22" s="55" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E22" s="54">
         <f t="shared" si="0"/>
@@ -4871,7 +4929,9 @@
       <c r="AG22" s="53"/>
       <c r="AH22" s="54"/>
       <c r="AI22" s="54"/>
-      <c r="AJ22" s="54"/>
+      <c r="AJ22" s="54">
+        <v>1</v>
+      </c>
       <c r="AK22" s="54"/>
       <c r="AL22" s="54"/>
       <c r="AM22" s="54"/>
@@ -4886,13 +4946,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C23" s="28">
         <v>13</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E23" s="57">
         <f t="shared" si="0"/>
@@ -4979,7 +5039,9 @@
       <c r="AG23" s="27"/>
       <c r="AH23" s="65"/>
       <c r="AI23" s="65"/>
-      <c r="AJ23" s="65"/>
+      <c r="AJ23" s="65">
+        <v>1</v>
+      </c>
       <c r="AK23" s="65"/>
       <c r="AL23" s="65"/>
       <c r="AM23" s="65"/>
@@ -4994,13 +5056,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="53" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C24" s="54">
         <v>35</v>
       </c>
       <c r="D24" s="55" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E24" s="54">
         <f t="shared" si="0"/>
@@ -5091,7 +5153,9 @@
       <c r="AG24" s="53"/>
       <c r="AH24" s="54"/>
       <c r="AI24" s="54"/>
-      <c r="AJ24" s="54"/>
+      <c r="AJ24" s="54">
+        <v>1</v>
+      </c>
       <c r="AK24" s="54"/>
       <c r="AL24" s="54"/>
       <c r="AM24" s="54"/>
@@ -5106,13 +5170,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="56" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C25" s="28">
         <v>43</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E25" s="57">
         <f t="shared" si="0"/>
@@ -5201,8 +5265,12 @@
       <c r="AG25" s="27"/>
       <c r="AH25" s="65"/>
       <c r="AI25" s="65"/>
-      <c r="AJ25" s="65"/>
-      <c r="AK25" s="65"/>
+      <c r="AJ25" s="65">
+        <v>1</v>
+      </c>
+      <c r="AK25" s="65">
+        <v>1</v>
+      </c>
       <c r="AL25" s="65"/>
       <c r="AM25" s="65"/>
       <c r="AN25" s="65"/>
@@ -5216,7 +5284,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="53" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C26" s="54">
         <v>0</v>
@@ -5309,8 +5377,12 @@
       <c r="AG26" s="53"/>
       <c r="AH26" s="54"/>
       <c r="AI26" s="54"/>
-      <c r="AJ26" s="54"/>
-      <c r="AK26" s="54"/>
+      <c r="AJ26" s="54">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="54">
+        <v>1</v>
+      </c>
       <c r="AL26" s="54"/>
       <c r="AM26" s="54"/>
       <c r="AN26" s="54"/>
@@ -5324,7 +5396,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="56" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C27" s="28">
         <v>0</v>
@@ -5417,8 +5489,12 @@
       <c r="AG27" s="27"/>
       <c r="AH27" s="65"/>
       <c r="AI27" s="65"/>
-      <c r="AJ27" s="65"/>
-      <c r="AK27" s="65"/>
+      <c r="AJ27" s="65">
+        <v>1</v>
+      </c>
+      <c r="AK27" s="65">
+        <v>1</v>
+      </c>
       <c r="AL27" s="65"/>
       <c r="AM27" s="65"/>
       <c r="AN27" s="65"/>
@@ -5438,7 +5514,7 @@
         <v>36</v>
       </c>
       <c r="D28" s="55" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E28" s="54">
         <f t="shared" si="0"/>
@@ -5531,7 +5607,9 @@
         <v>1</v>
       </c>
       <c r="AI28" s="54"/>
-      <c r="AJ28" s="54"/>
+      <c r="AJ28" s="54">
+        <v>1</v>
+      </c>
       <c r="AK28" s="54"/>
       <c r="AL28" s="54"/>
       <c r="AM28" s="54"/>
@@ -5552,7 +5630,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E29" s="57">
         <f t="shared" si="0"/>
@@ -5637,7 +5715,9 @@
       <c r="AI29" s="65">
         <v>1</v>
       </c>
-      <c r="AJ29" s="65"/>
+      <c r="AJ29" s="65">
+        <v>1</v>
+      </c>
       <c r="AK29" s="65"/>
       <c r="AL29" s="65"/>
       <c r="AM29" s="65"/>
@@ -8815,7 +8895,7 @@
   </sheetPr>
   <dimension ref="A1:AX67"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="AF62" sqref="AF62"/>
@@ -8896,7 +8976,7 @@
         <v>F0</v>
       </c>
       <c r="P1" s="32" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q1" s="37" t="str">
         <f>真值表!R1</f>
@@ -8972,11 +9052,11 @@
       </c>
       <c r="AI1" s="42" t="str">
         <f>真值表!AJ1</f>
-        <v>XXX</v>
+        <v>R1_Used</v>
       </c>
       <c r="AJ1" s="42" t="str">
         <f>真值表!AK1</f>
-        <v>XXX</v>
+        <v>R2_Used</v>
       </c>
       <c r="AK1" s="42" t="str">
         <f>真值表!AL1</f>
@@ -9150,7 +9230,7 @@
       </c>
       <c r="AJ2" s="38" t="str">
         <f>IF(真值表!AK2=1,$P2&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AK2" s="38" t="str">
         <f>IF(真值表!AL2=1,$P2&amp;"+","")</f>
@@ -9324,7 +9404,7 @@
       </c>
       <c r="AJ3" s="39" t="str">
         <f>IF(真值表!AK3=1,$P3&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AK3" s="39" t="str">
         <f>IF(真值表!AL3=1,$P3&amp;"+","")</f>
@@ -9498,7 +9578,7 @@
       </c>
       <c r="AJ4" s="38" t="str">
         <f>IF(真值表!AK4=1,$P4&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AK4" s="38" t="str">
         <f>IF(真值表!AL4=1,$P4&amp;"+","")</f>
@@ -9668,11 +9748,11 @@
       </c>
       <c r="AI5" s="39" t="str">
         <f>IF(真值表!AJ5=1,$P5&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AJ5" s="39" t="str">
         <f>IF(真值表!AK5=1,$P5&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AK5" s="39" t="str">
         <f>IF(真值表!AL5=1,$P5&amp;"+","")</f>
@@ -9842,11 +9922,11 @@
       </c>
       <c r="AI6" s="38" t="str">
         <f>IF(真值表!AJ6=1,$P6&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AJ6" s="38" t="str">
         <f>IF(真值表!AK6=1,$P6&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AK6" s="38" t="str">
         <f>IF(真值表!AL6=1,$P6&amp;"+","")</f>
@@ -10016,11 +10096,11 @@
       </c>
       <c r="AI7" s="39" t="str">
         <f>IF(真值表!AJ7=1,$P7&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AJ7" s="39" t="str">
         <f>IF(真值表!AK7=1,$P7&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AK7" s="39" t="str">
         <f>IF(真值表!AL7=1,$P7&amp;"+","")</f>
@@ -10190,11 +10270,11 @@
       </c>
       <c r="AI8" s="38" t="str">
         <f>IF(真值表!AJ8=1,$P8&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AJ8" s="38" t="str">
         <f>IF(真值表!AK8=1,$P8&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AK8" s="38" t="str">
         <f>IF(真值表!AL8=1,$P8&amp;"+","")</f>
@@ -10364,11 +10444,11 @@
       </c>
       <c r="AI9" s="39" t="str">
         <f>IF(真值表!AJ9=1,$P9&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AJ9" s="39" t="str">
         <f>IF(真值表!AK9=1,$P9&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AK9" s="39" t="str">
         <f>IF(真值表!AL9=1,$P9&amp;"+","")</f>
@@ -10538,11 +10618,11 @@
       </c>
       <c r="AI10" s="38" t="str">
         <f>IF(真值表!AJ10=1,$P10&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AJ10" s="38" t="str">
         <f>IF(真值表!AK10=1,$P10&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AK10" s="38" t="str">
         <f>IF(真值表!AL10=1,$P10&amp;"+","")</f>
@@ -10712,11 +10792,11 @@
       </c>
       <c r="AI11" s="39" t="str">
         <f>IF(真值表!AJ11=1,$P11&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AJ11" s="39" t="str">
         <f>IF(真值表!AK11=1,$P11&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AK11" s="39" t="str">
         <f>IF(真值表!AL11=1,$P11&amp;"+","")</f>
@@ -10886,11 +10966,11 @@
       </c>
       <c r="AI12" s="38" t="str">
         <f>IF(真值表!AJ12=1,$P12&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AJ12" s="38" t="str">
         <f>IF(真值表!AK12=1,$P12&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AK12" s="38" t="str">
         <f>IF(真值表!AL12=1,$P12&amp;"+","")</f>
@@ -11060,7 +11140,7 @@
       </c>
       <c r="AI13" s="39" t="str">
         <f>IF(真值表!AJ13=1,$P13&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AJ13" s="39" t="str">
         <f>IF(真值表!AK13=1,$P13&amp;"+","")</f>
@@ -11234,11 +11314,11 @@
       </c>
       <c r="AI14" s="38" t="str">
         <f>IF(真值表!AJ14=1,$P14&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AJ14" s="38" t="str">
         <f>IF(真值表!AK14=1,$P14&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AK14" s="38" t="str">
         <f>IF(真值表!AL14=1,$P14&amp;"+","")</f>
@@ -11756,11 +11836,11 @@
       </c>
       <c r="AI17" s="39" t="str">
         <f>IF(真值表!AJ17=1,$P17&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AJ17" s="39" t="str">
         <f>IF(真值表!AK17=1,$P17&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AK17" s="39" t="str">
         <f>IF(真值表!AL17=1,$P17&amp;"+","")</f>
@@ -11930,11 +12010,11 @@
       </c>
       <c r="AI18" s="38" t="str">
         <f>IF(真值表!AJ18=1,$P18&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AJ18" s="38" t="str">
         <f>IF(真值表!AK18=1,$P18&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AK18" s="38" t="str">
         <f>IF(真值表!AL18=1,$P18&amp;"+","")</f>
@@ -12104,7 +12184,7 @@
       </c>
       <c r="AI19" s="39" t="str">
         <f>IF(真值表!AJ19=1,$P19&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AJ19" s="39" t="str">
         <f>IF(真值表!AK19=1,$P19&amp;"+","")</f>
@@ -12278,7 +12358,7 @@
       </c>
       <c r="AI20" s="38" t="str">
         <f>IF(真值表!AJ20=1,$P20&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AJ20" s="38" t="str">
         <f>IF(真值表!AK20=1,$P20&amp;"+","")</f>
@@ -12452,7 +12532,7 @@
       </c>
       <c r="AI21" s="39" t="str">
         <f>IF(真值表!AJ21=1,$P21&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AJ21" s="39" t="str">
         <f>IF(真值表!AK21=1,$P21&amp;"+","")</f>
@@ -12626,7 +12706,7 @@
       </c>
       <c r="AI22" s="38" t="str">
         <f>IF(真值表!AJ22=1,$P22&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="AJ22" s="38" t="str">
         <f>IF(真值表!AK22=1,$P22&amp;"+","")</f>
@@ -12800,7 +12880,7 @@
       </c>
       <c r="AI23" s="39" t="str">
         <f>IF(真值表!AJ23=1,$P23&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AJ23" s="39" t="str">
         <f>IF(真值表!AK23=1,$P23&amp;"+","")</f>
@@ -12974,7 +13054,7 @@
       </c>
       <c r="AI24" s="38" t="str">
         <f>IF(真值表!AJ24=1,$P24&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AJ24" s="38" t="str">
         <f>IF(真值表!AK24=1,$P24&amp;"+","")</f>
@@ -13148,11 +13228,11 @@
       </c>
       <c r="AI25" s="39" t="str">
         <f>IF(真值表!AJ25=1,$P25&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AJ25" s="39" t="str">
         <f>IF(真值表!AK25=1,$P25&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AK25" s="39" t="str">
         <f>IF(真值表!AL25=1,$P25&amp;"+","")</f>
@@ -13322,11 +13402,11 @@
       </c>
       <c r="AI26" s="38" t="str">
         <f>IF(真值表!AJ26=1,$P26&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AJ26" s="38" t="str">
         <f>IF(真值表!AK26=1,$P26&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AK26" s="38" t="str">
         <f>IF(真值表!AL26=1,$P26&amp;"+","")</f>
@@ -13496,11 +13576,11 @@
       </c>
       <c r="AI27" s="39" t="str">
         <f>IF(真值表!AJ27=1,$P27&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AJ27" s="39" t="str">
         <f>IF(真值表!AK27=1,$P27&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AK27" s="39" t="str">
         <f>IF(真值表!AL27=1,$P27&amp;"+","")</f>
@@ -13670,7 +13750,7 @@
       </c>
       <c r="AI28" s="38" t="str">
         <f>IF(真值表!AJ28=1,$P28&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AJ28" s="38" t="str">
         <f>IF(真值表!AK28=1,$P28&amp;"+","")</f>
@@ -13844,7 +13924,7 @@
       </c>
       <c r="AI29" s="39" t="str">
         <f>IF(真值表!AJ29=1,$P29&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AJ29" s="39" t="str">
         <f>IF(真值表!AK29=1,$P29&amp;"+","")</f>
@@ -19449,7 +19529,7 @@
     </row>
     <row r="62" ht="16.2" spans="1:43">
       <c r="A62" s="31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B62" s="31"/>
       <c r="C62" s="31"/>
@@ -19540,11 +19620,11 @@
       </c>
       <c r="AI62" s="41" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp; OP0</v>
       </c>
       <c r="AJ62" s="41" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0</v>
       </c>
       <c r="AK62" s="41" t="str">
         <f t="shared" si="1"/>
@@ -19650,11 +19730,11 @@
       </c>
       <c r="AI63" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AJ63" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AK63" t="str">
         <f t="shared" si="2"/>
@@ -19715,7 +19795,7 @@
     </row>
     <row r="65" ht="20.4" spans="22:32">
       <c r="V65" s="43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="W65" s="43"/>
       <c r="X65" s="43"/>
@@ -19730,7 +19810,7 @@
     </row>
     <row r="67" ht="16.2" spans="18:18">
       <c r="R67" s="44" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -19803,98 +19883,98 @@
         <v>16</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" ht="18" customHeight="1" spans="1:3">
       <c r="A2" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B2" s="12">
         <v>0</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1" spans="1:3">
       <c r="A3" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" s="12">
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" ht="18" customHeight="1" spans="1:3">
       <c r="A4" s="11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" s="12">
         <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" ht="18" customHeight="1" spans="1:3">
       <c r="A5" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B5" s="12">
         <v>3</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" ht="18" customHeight="1" spans="1:3">
       <c r="A6" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B6" s="12">
         <v>4</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" ht="18" customHeight="1" spans="1:3">
       <c r="A7" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B7" s="12">
         <v>5</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" ht="18" customHeight="1" spans="1:3">
       <c r="A8" s="11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B8" s="12">
         <v>6</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" ht="18" customHeight="1" spans="1:3">
       <c r="A9" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B9" s="12">
         <v>7</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" ht="18" customHeight="1" spans="1:3">
@@ -19905,7 +19985,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" ht="18" customHeight="1" spans="1:3">
@@ -19916,7 +19996,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" ht="18" customHeight="1" spans="1:3">
@@ -19927,7 +20007,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:3">
@@ -19938,7 +20018,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:3">
@@ -19949,7 +20029,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" ht="14.55"/>
@@ -19982,13 +20062,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -19999,10 +20079,10 @@
         <v>24</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20013,10 +20093,10 @@
         <v>22</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20024,13 +20104,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20038,13 +20118,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20055,10 +20135,10 @@
         <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20066,13 +20146,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20083,10 +20163,10 @@
         <v>26</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20097,10 +20177,10 @@
         <v>30</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20111,10 +20191,10 @@
         <v>32</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20125,10 +20205,10 @@
         <v>31</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20136,13 +20216,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20150,13 +20230,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" ht="20.1" customHeight="1" spans="1:4">
@@ -20164,13 +20244,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BEQ,BNE is signExt, have debug it
</commit_message>
<xml_diff>
--- a/CPU28/单周期控制器2020-2-14.xlsx
+++ b/CPU28/单周期控制器2020-2-14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16331" windowHeight="9684"/>
+    <workbookView windowWidth="16331" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="真值表" sheetId="1" r:id="rId1"/>
@@ -842,10 +842,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="51">
     <font>
@@ -1013,16 +1013,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1033,38 +1049,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1080,7 +1073,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1088,9 +1088,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1102,19 +1102,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1127,22 +1134,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1151,6 +1143,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1267,7 +1267,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1279,43 +1399,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1327,97 +1417,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1435,13 +1441,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1631,10 +1631,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1643,8 +1641,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1660,6 +1658,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1690,24 +1703,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1732,10 +1732,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1744,133 +1744,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="23" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="28" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="18" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2454,8 +2454,8 @@
   </sheetPr>
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AL13" sqref="AL13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -4360,7 +4360,9 @@
       <c r="X17" s="27"/>
       <c r="Y17" s="27"/>
       <c r="Z17" s="27"/>
-      <c r="AA17" s="27"/>
+      <c r="AA17" s="27">
+        <v>1</v>
+      </c>
       <c r="AB17" s="27"/>
       <c r="AC17" s="27">
         <v>1</v>
@@ -4470,7 +4472,9 @@
       <c r="X18" s="53"/>
       <c r="Y18" s="53"/>
       <c r="Z18" s="53"/>
-      <c r="AA18" s="53"/>
+      <c r="AA18" s="53">
+        <v>1</v>
+      </c>
       <c r="AB18" s="53"/>
       <c r="AC18" s="53"/>
       <c r="AD18" s="53">
@@ -5704,7 +5708,9 @@
       <c r="X29" s="27"/>
       <c r="Y29" s="27"/>
       <c r="Z29" s="27"/>
-      <c r="AA29" s="27"/>
+      <c r="AA29" s="27">
+        <v>1</v>
+      </c>
       <c r="AB29" s="27"/>
       <c r="AC29" s="27"/>
       <c r="AD29" s="27"/>
@@ -11800,7 +11806,7 @@
       </c>
       <c r="Z17" s="39" t="str">
         <f>IF(真值表!AA17=1,$P17&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AA17" s="39" t="str">
         <f>IF(真值表!AB17=1,$P17&amp;"+","")</f>
@@ -11974,7 +11980,7 @@
       </c>
       <c r="Z18" s="38" t="str">
         <f>IF(真值表!AA18=1,$P18&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AA18" s="38" t="str">
         <f>IF(真值表!AB18=1,$P18&amp;"+","")</f>
@@ -13888,7 +13894,7 @@
       </c>
       <c r="Z29" s="39" t="str">
         <f>IF(真值表!AA29=1,$P29&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AA29" s="39" t="str">
         <f>IF(真值表!AB29=1,$P29&amp;"+","")</f>
@@ -19584,7 +19590,7 @@
       </c>
       <c r="Z62" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp; OP0</v>
       </c>
       <c r="AA62" s="41" t="str">
         <f t="shared" si="1"/>
@@ -19694,7 +19700,7 @@
       </c>
       <c r="Z63" t="str">
         <f t="shared" si="2"/>
-        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AA63" t="str">
         <f t="shared" si="2"/>

</xml_diff>